<commit_message>
updated august and september
</commit_message>
<xml_diff>
--- a/data/Production_Filled_June.xlsx
+++ b/data/Production_Filled_June.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cil94\Desktop\test\Filter_form\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cil94\Desktop\Filter_form\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8340" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="108">
   <si>
     <t>DATE</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>WITH OUT TAW ROLL PROD.</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t xml:space="preserve">14/10 &amp; 36 lbs SALE YARN </t>
@@ -6555,8 +6552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT27"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN10" sqref="AN10"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ15" sqref="AJ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6586,106 +6583,106 @@
         <v>11</v>
       </c>
       <c r="G1" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="K1" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="N1" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="O1" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="38" t="s">
+      <c r="P1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="U1" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="32" t="s">
+      <c r="V1" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="V1" s="32" t="s">
+      <c r="W1" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="W1" s="32" t="s">
+      <c r="X1" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="X1" s="32" t="s">
+      <c r="Y1" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="Y1" s="37" t="s">
+      <c r="Z1" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="Z1" s="32" t="s">
+      <c r="AA1" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="AA1" s="32" t="s">
+      <c r="AB1" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="AB1" s="32" t="s">
+      <c r="AC1" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="AC1" s="32" t="s">
+      <c r="AD1" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="AD1" s="37" t="s">
+      <c r="AE1" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="AE1" s="32" t="s">
+      <c r="AF1" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="AF1" s="32" t="s">
+      <c r="AG1" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="AG1" s="32" t="s">
+      <c r="AH1" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="AH1" s="32" t="s">
+      <c r="AI1" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="AI1" s="37" t="s">
+      <c r="AJ1" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="AJ1" s="32" t="s">
+      <c r="AK1" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="AK1" s="32" t="s">
+      <c r="AL1" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="AL1" s="32" t="s">
+      <c r="AM1" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="AM1" s="32" t="s">
+      <c r="AN1" s="37" t="s">
         <v>107</v>
-      </c>
-      <c r="AN1" s="37" t="s">
-        <v>108</v>
       </c>
       <c r="AO1" s="36" t="s">
         <v>3</v>
@@ -9260,7 +9257,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9284,7 +9281,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>11</v>
@@ -9425,17 +9422,17 @@
       <c r="A7" s="2">
         <v>45815</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>14</v>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="14">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="0"/>
@@ -9727,14 +9724,14 @@
       <c r="B19" s="3">
         <v>0</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>14</v>
+      <c r="C19" s="14">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
@@ -9980,7 +9977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
     </sheetView>
@@ -10080,7 +10077,7 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3">
         <v>37.707999999999998</v>
@@ -10157,7 +10154,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4">
         <v>2.3559999999999999</v>
@@ -10235,7 +10232,7 @@
     <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3">
         <f t="shared" ref="B6:AA6" si="0">B2+B3</f>
@@ -10344,14 +10341,14 @@
     </row>
     <row r="8" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I8" s="22"/>
       <c r="M8" s="22"/>
     </row>
     <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="23">
         <v>128</v>
@@ -10430,7 +10427,7 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3">
         <v>1.4</v>
@@ -10463,7 +10460,7 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3">
         <v>0.2</v>
@@ -10510,7 +10507,7 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3">
         <v>0.82099999999999995</v>
@@ -10589,7 +10586,7 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="3">
         <v>18.334</v>
@@ -10668,7 +10665,7 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -10717,7 +10714,7 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
@@ -10750,7 +10747,7 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -10815,7 +10812,7 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="3">
         <v>12.34</v>
@@ -10897,7 +10894,7 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="3">
         <v>1.956</v>
@@ -10962,7 +10959,7 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -10993,7 +10990,7 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -11050,7 +11047,7 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -11081,7 +11078,7 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -11120,7 +11117,7 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -11163,7 +11160,7 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="3">
         <v>2.1219999999999999</v>
@@ -11230,7 +11227,7 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="3">
         <v>1.01</v>
@@ -11441,7 +11438,7 @@
     <row r="29" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="4">
         <f t="shared" ref="B30:AA30" si="3">B6-B28</f>
@@ -11550,14 +11547,14 @@
     </row>
     <row r="32" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="40"/>
       <c r="C32" s="40"/>
     </row>
     <row r="33" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="3">
         <v>0.79300000000000004</v>
@@ -11637,7 +11634,7 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" s="4">
         <f t="shared" ref="B35:AA35" si="4">SUM(B33:B34)</f>
@@ -11746,14 +11743,14 @@
     </row>
     <row r="37" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" s="40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" s="40"/>
       <c r="C37" s="40"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" s="3">
         <v>2.218</v>
@@ -11838,7 +11835,7 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -11879,7 +11876,7 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" s="3">
         <v>24.364000000000001</v>
@@ -11958,7 +11955,7 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B41" s="3">
         <v>3.11</v>
@@ -12037,7 +12034,7 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" s="3">
         <v>0.45100000000000001</v>
@@ -12116,7 +12113,7 @@
     </row>
     <row r="43" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B43" s="3">
         <v>0.13300000000000001</v>
@@ -12197,7 +12194,7 @@
     <row r="45" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B46" s="4">
         <f>SUM(B37:B44)</f>
@@ -12307,7 +12304,7 @@
     <row r="47" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B48" s="4">
         <f t="shared" ref="B48:AA48" si="6">B28-B35-B46</f>
@@ -12419,7 +12416,7 @@
     </row>
     <row r="51" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A51" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B51" s="40"/>
       <c r="C51" s="40"/>
@@ -12449,7 +12446,7 @@
     </row>
     <row r="52" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B52" s="3">
         <v>0</v>
@@ -12526,7 +12523,7 @@
     </row>
     <row r="53" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B53" s="3">
         <v>13.5</v>
@@ -12603,7 +12600,7 @@
     </row>
     <row r="54" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B54" s="3">
         <v>0.6</v>
@@ -12680,7 +12677,7 @@
     </row>
     <row r="55" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B55" s="3">
         <v>15.5</v>
@@ -12757,7 +12754,7 @@
     </row>
     <row r="56" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B56" s="3">
         <v>2.5</v>
@@ -12834,7 +12831,7 @@
     </row>
     <row r="57" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B57" s="3">
         <v>151.34800000000001</v>
@@ -12911,7 +12908,7 @@
     </row>
     <row r="58" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B58" s="3">
         <v>3</v>
@@ -12986,7 +12983,7 @@
     </row>
     <row r="59" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -13017,7 +13014,7 @@
     </row>
     <row r="60" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B60" s="3">
         <v>56.957000000000001</v>
@@ -13094,7 +13091,7 @@
     </row>
     <row r="61" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3">
@@ -13169,7 +13166,7 @@
     </row>
     <row r="62" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B62" s="3">
         <v>0</v>
@@ -13202,7 +13199,7 @@
     </row>
     <row r="63" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63" s="3">
         <v>0</v>
@@ -13279,7 +13276,7 @@
     </row>
     <row r="64" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -13310,7 +13307,7 @@
     </row>
     <row r="65" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B65" s="3">
         <v>5</v>
@@ -13387,7 +13384,7 @@
     </row>
     <row r="66" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B66" s="3">
         <v>2</v>
@@ -13629,7 +13626,7 @@
     </row>
     <row r="70" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="3">
@@ -13791,7 +13788,7 @@
     </row>
     <row r="73" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A73" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B73" s="40"/>
       <c r="C73" s="40"/>
@@ -13821,7 +13818,7 @@
     </row>
     <row r="74" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B74" s="3">
         <v>2.4</v>
@@ -13898,7 +13895,7 @@
     </row>
     <row r="75" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B75" s="3">
         <v>0</v>
@@ -13975,7 +13972,7 @@
     </row>
     <row r="76" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B76" s="3">
         <v>4.3499999999999996</v>
@@ -14052,7 +14049,7 @@
     </row>
     <row r="77" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B77" s="3">
         <v>0</v>
@@ -14129,7 +14126,7 @@
     </row>
     <row r="78" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B78" s="3">
         <v>10.02</v>
@@ -14206,7 +14203,7 @@
     </row>
     <row r="79" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B79" s="3">
         <v>0</v>
@@ -14283,7 +14280,7 @@
     </row>
     <row r="80" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3">
@@ -14358,7 +14355,7 @@
     </row>
     <row r="81" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B81" s="3">
         <v>0.72</v>
@@ -14427,7 +14424,7 @@
     </row>
     <row r="82" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B82" s="3">
         <v>1.335</v>
@@ -14504,7 +14501,7 @@
     </row>
     <row r="83" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B83" s="3">
         <v>0.78</v>
@@ -14746,7 +14743,7 @@
     </row>
     <row r="87" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3">
@@ -14880,7 +14877,7 @@
     </row>
     <row r="89" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B89" s="3">
         <f t="shared" ref="B89:AA89" si="12">+B69+B86</f>
@@ -15017,7 +15014,7 @@
     </row>
     <row r="91" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="3">

</xml_diff>